<commit_message>
Commit all files except Excel files
</commit_message>
<xml_diff>
--- a/przykladowe_dane_sparing_wiecej.xlsx
+++ b/przykladowe_dane_sparing_wiecej.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wojciechpyzel/Desktop/PROJEKTY/KODOWANIE/SPARING/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC05AD2-6E39-1C40-9D74-4ED1CEC00B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A658DD0-2198-044F-B1CC-C901FBCACE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="25700" windowHeight="15040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16540" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>